<commit_message>
linked plannification to database with calculations
</commit_message>
<xml_diff>
--- a/mysite/prevision.xlsx
+++ b/mysite/prevision.xlsx
@@ -466,7 +466,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="n">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5">
@@ -490,7 +490,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="n">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="8">
@@ -506,7 +506,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="n">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="10">
@@ -522,7 +522,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="n">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="12">
@@ -530,7 +530,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="n">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="13">
@@ -538,7 +538,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="n">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="14">
@@ -546,7 +546,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="n">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="15">
@@ -554,7 +554,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="n">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="16">
@@ -562,7 +562,7 @@
         <v>15</v>
       </c>
       <c r="B16" t="n">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="17">
@@ -586,7 +586,7 @@
         <v>18</v>
       </c>
       <c r="B19" t="n">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="20">
@@ -618,7 +618,7 @@
         <v>22</v>
       </c>
       <c r="B23" t="n">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="24">
@@ -634,7 +634,7 @@
         <v>24</v>
       </c>
       <c r="B25" t="n">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="26">
@@ -650,7 +650,7 @@
         <v>26</v>
       </c>
       <c r="B27" t="n">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="28">
@@ -666,7 +666,7 @@
         <v>28</v>
       </c>
       <c r="B29" t="n">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="30">
@@ -674,7 +674,7 @@
         <v>29</v>
       </c>
       <c r="B30" t="n">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="31">
@@ -698,7 +698,7 @@
         <v>32</v>
       </c>
       <c r="B33" t="n">
-        <v>58</v>
+        <v>60</v>
       </c>
     </row>
     <row r="34">
@@ -706,7 +706,7 @@
         <v>33</v>
       </c>
       <c r="B34" t="n">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="35">
@@ -714,7 +714,7 @@
         <v>34</v>
       </c>
       <c r="B35" t="n">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="36">
@@ -738,7 +738,7 @@
         <v>37</v>
       </c>
       <c r="B38" t="n">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="39">
@@ -754,7 +754,7 @@
         <v>39</v>
       </c>
       <c r="B40" t="n">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="41">
@@ -762,7 +762,7 @@
         <v>40</v>
       </c>
       <c r="B41" t="n">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="42">
@@ -770,7 +770,7 @@
         <v>41</v>
       </c>
       <c r="B42" t="n">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="43">
@@ -802,7 +802,7 @@
         <v>45</v>
       </c>
       <c r="B46" t="n">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="47">
@@ -810,7 +810,7 @@
         <v>46</v>
       </c>
       <c r="B47" t="n">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="48">
@@ -834,7 +834,7 @@
         <v>49</v>
       </c>
       <c r="B50" t="n">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="51">
@@ -842,7 +842,7 @@
         <v>50</v>
       </c>
       <c r="B51" t="n">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="52">
@@ -850,7 +850,7 @@
         <v>51</v>
       </c>
       <c r="B52" t="n">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="53">
@@ -858,7 +858,7 @@
         <v>52</v>
       </c>
       <c r="B53" t="n">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>